<commit_message>
Good find on Frequency function
</commit_message>
<xml_diff>
--- a/FrequencyFunctionExperiment.xlsx
+++ b/FrequencyFunctionExperiment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1BD8624-5283-440E-8AB7-C3D66FADBC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00AB7176-E258-4E22-BDB4-FA2C9DD4E6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62685" yWindow="555" windowWidth="21600" windowHeight="12675" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>FROM:</t>
   </si>
@@ -77,6 +77,48 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>Frequency Table</t>
+  </si>
+  <si>
+    <t>&lt;=24</t>
+  </si>
+  <si>
+    <t>(24,25]</t>
+  </si>
+  <si>
+    <t>(25,26]</t>
+  </si>
+  <si>
+    <t>(26,27]</t>
+  </si>
+  <si>
+    <t>&gt;27</t>
+  </si>
+  <si>
+    <t>Another View</t>
+  </si>
+  <si>
+    <t>Initial Concept</t>
+  </si>
+  <si>
+    <t>"Negative" Frequency Table</t>
+  </si>
+  <si>
+    <t>&lt;24</t>
+  </si>
+  <si>
+    <t>[25,26)</t>
+  </si>
+  <si>
+    <t>[24,25)</t>
+  </si>
+  <si>
+    <t>[26,27)</t>
+  </si>
+  <si>
+    <t>&gt;=27</t>
   </si>
 </sst>
 </file>
@@ -168,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +244,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,12 +315,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -375,6 +448,13 @@
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFF99"/>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFCCCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -574,13 +654,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="1.77734375" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="11" max="11" width="1.77734375" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -591,6 +677,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -601,6 +688,7 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -612,6 +700,12 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -692,19 +786,254 @@
         <v>2.9999989999999999</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C17" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C18" s="3">
         <v>3.2</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C19" s="3">
         <v>3.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E26" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E27)</f>
+        <v>=FREQUENCY(B28:B41,C28:C31)</v>
+      </c>
+      <c r="J26" t="s">
+        <v>5</v>
+      </c>
+      <c r="L26" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(L27)</f>
+        <v>=DROP(FREQUENCY(-I28:I41,-J27:J31),-1)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" cm="1">
+        <f t="array" ref="E27:E31">FREQUENCY(B28:B41,C28:C31)</f>
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>6</v>
+      </c>
+      <c r="L27" cm="1">
+        <f t="array" ref="L27:L31">_xlfn.DROP(FREQUENCY(-I28:I41,-J27:J31),-1)</f>
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>24</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="11">
+        <v>23.9</v>
+      </c>
+      <c r="J28">
+        <v>24</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="10">
+        <v>24.0001</v>
+      </c>
+      <c r="C29">
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <v>8</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="10">
+        <v>24</v>
+      </c>
+      <c r="J29">
+        <v>25</v>
+      </c>
+      <c r="L29">
+        <v>7</v>
+      </c>
+      <c r="M29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="10">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>26</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="10">
+        <v>24.99</v>
+      </c>
+      <c r="J30">
+        <v>26</v>
+      </c>
+      <c r="L30">
+        <v>2</v>
+      </c>
+      <c r="M30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="9">
+        <v>25.3</v>
+      </c>
+      <c r="C31">
+        <v>27</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="9">
+        <v>25</v>
+      </c>
+      <c r="J31">
+        <v>27</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="9">
+        <v>25.4</v>
+      </c>
+      <c r="I32" s="9">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="9">
+        <v>25.5</v>
+      </c>
+      <c r="I33" s="9">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="9">
+        <v>25.6</v>
+      </c>
+      <c r="I34" s="9">
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="9">
+        <v>25.7</v>
+      </c>
+      <c r="I35" s="9">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="9">
+        <v>25.8</v>
+      </c>
+      <c r="I36" s="9">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="9">
+        <v>25.9</v>
+      </c>
+      <c r="I37" s="9">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="9">
+        <v>26</v>
+      </c>
+      <c r="I38" s="8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="8">
+        <v>26.5</v>
+      </c>
+      <c r="I39" s="8">
+        <v>26.99</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="7">
+        <v>27.00001</v>
+      </c>
+      <c r="I40" s="7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="7">
+        <v>29</v>
+      </c>
+      <c r="I41" s="7">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>